<commit_message>
models results and figure oil exploration updated
</commit_message>
<xml_diff>
--- a/results/MCMC_model results .xlsx
+++ b/results/MCMC_model results .xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
-  <workbookPr defaultThemeVersion="202300"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unioviedo-my.sharepoint.com/personal/espinosaclara_uniovi_es/Documents/IMIB/Softwares/GitHub/Oilcontent_Longevity/results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laptop\OneDrive - Universidad de Oviedo\IMIB\Softwares\GitHub\Oilcontent_Longevity\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="166" documentId="8_{39778DF2-0EA2-4210-9915-5D157E3CC058}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C89BBB48-5E1F-4D7D-BEAB-AF07705FB039}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3B26452E-8955-468B-B3A8-3BA11867AC14}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
-    <sheet name="MCMC" sheetId="1" r:id="rId1"/>
+    <sheet name="MCMC_dec24" sheetId="2" r:id="rId1"/>
+    <sheet name="MCMC" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="113">
   <si>
     <t>FDD</t>
   </si>
@@ -231,13 +231,157 @@
   </si>
   <si>
     <t>Loil.content</t>
+  </si>
+  <si>
+    <t>ecology (low vs gen vs alp)</t>
+  </si>
+  <si>
+    <t>Loil_content ~ ecology</t>
+  </si>
+  <si>
+    <t>ecologyGeneralist</t>
+  </si>
+  <si>
+    <t>ecologyStrict alpine</t>
+  </si>
+  <si>
+    <t>(Intercept) Strict Lowland</t>
+  </si>
+  <si>
+    <t>Seed mass (log)</t>
+  </si>
+  <si>
+    <t>Loil_content ~ Lseed_mass</t>
+  </si>
+  <si>
+    <t>~ animal + ID</t>
+  </si>
+  <si>
+    <t>MODEL name</t>
+  </si>
+  <si>
+    <t>g1</t>
+  </si>
+  <si>
+    <t>g2</t>
+  </si>
+  <si>
+    <t>g3</t>
+  </si>
+  <si>
+    <t>g4</t>
+  </si>
+  <si>
+    <t>Model name</t>
+  </si>
+  <si>
+    <t>Seed mass (log) (n=49)</t>
+  </si>
+  <si>
+    <t>Own oil data (n= 47 species, 49 accessions)</t>
+  </si>
+  <si>
+    <t>Own oil data + literature (n= 80 species, 82 accessions)</t>
+  </si>
+  <si>
+    <t>m1</t>
+  </si>
+  <si>
+    <t>m2</t>
+  </si>
+  <si>
+    <t>Longevity curves (n=31)</t>
+  </si>
+  <si>
+    <t>&lt; 1e-04</t>
+  </si>
+  <si>
+    <t>g5</t>
+  </si>
+  <si>
+    <t>g6</t>
+  </si>
+  <si>
+    <t>p50 (square rooted) (n=33)</t>
+  </si>
+  <si>
+    <t>T50_mean ~Loil.content</t>
+  </si>
+  <si>
+    <t>EHS (log) (n= 36)</t>
+  </si>
+  <si>
+    <t>Lp50 ~  Lratio</t>
+  </si>
+  <si>
+    <t>T50_mean ~Lratio</t>
+  </si>
+  <si>
+    <t>LEHS_mean ~Loil.content</t>
+  </si>
+  <si>
+    <t>LEHS_mean ~ratio</t>
+  </si>
+  <si>
+    <t>Lratio ~ Lseedmass</t>
+  </si>
+  <si>
+    <t>T50 (n= 36) convex distribution</t>
+  </si>
+  <si>
+    <t>g7</t>
+  </si>
+  <si>
+    <t>g8</t>
+  </si>
+  <si>
+    <t>g9</t>
+  </si>
+  <si>
+    <t>g10</t>
+  </si>
+  <si>
+    <t>Strict alpine</t>
+  </si>
+  <si>
+    <t>g11</t>
+  </si>
+  <si>
+    <t>g12</t>
+  </si>
+  <si>
+    <t>Loil.content ~GDD</t>
+  </si>
+  <si>
+    <t>Lratio  ~ GDD</t>
+  </si>
+  <si>
+    <t>g13</t>
+  </si>
+  <si>
+    <t>g14</t>
+  </si>
+  <si>
+    <t>g15</t>
+  </si>
+  <si>
+    <t>g16</t>
+  </si>
+  <si>
+    <t>Loil.content ~ FDD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lratio  ~ FDD </t>
+  </si>
+  <si>
+    <t>Lratio ~ ecology</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -271,16 +415,60 @@
       <name val="Lucida Console"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Lucida Sans Typewriter"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="17">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -506,11 +694,204 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -558,35 +939,178 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -925,33 +1449,1160 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B031E22A-FA56-4347-B0C3-82A7571EE57F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:M32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="68.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="10.75" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="21" customHeight="1" thickBot="1">
+      <c r="A1" s="71" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="72"/>
+      <c r="I1" s="72"/>
+      <c r="J1" s="72"/>
+      <c r="K1" s="72"/>
+      <c r="L1" s="72"/>
+      <c r="M1" s="73"/>
+    </row>
+    <row r="2" spans="1:13" s="42" customFormat="1" ht="16.5" thickBot="1">
+      <c r="A2" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="39" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" s="40" t="s">
+        <v>36</v>
+      </c>
+      <c r="J2" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="K2" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="L2" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="M2" s="48" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" s="44" customFormat="1" ht="15">
+      <c r="A3" s="52" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="52" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="53" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="53" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" s="53" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="54" t="s">
+        <v>69</v>
+      </c>
+      <c r="H3" s="55">
+        <v>2.1250909999999998</v>
+      </c>
+      <c r="I3" s="55">
+        <v>1.4455420000000001</v>
+      </c>
+      <c r="J3" s="55">
+        <v>2.8028209999999998</v>
+      </c>
+      <c r="K3" s="55">
+        <v>9000</v>
+      </c>
+      <c r="L3" s="55" t="s">
+        <v>2</v>
+      </c>
+      <c r="M3" s="56" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" s="44" customFormat="1" ht="15">
+      <c r="A4" s="57"/>
+      <c r="B4" s="57"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="50" t="s">
+        <v>67</v>
+      </c>
+      <c r="H4" s="51">
+        <v>-8.9210000000000001E-3</v>
+      </c>
+      <c r="I4" s="51">
+        <v>-0.28595799999999999</v>
+      </c>
+      <c r="J4" s="51">
+        <v>0.25387199999999999</v>
+      </c>
+      <c r="K4" s="51">
+        <v>8661</v>
+      </c>
+      <c r="L4" s="51">
+        <v>0.94699999999999995</v>
+      </c>
+      <c r="M4" s="58"/>
+    </row>
+    <row r="5" spans="1:13" s="44" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A5" s="59"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="61" t="s">
+        <v>68</v>
+      </c>
+      <c r="H5" s="62">
+        <v>-0.107848</v>
+      </c>
+      <c r="I5" s="62">
+        <v>-0.41161500000000001</v>
+      </c>
+      <c r="J5" s="62">
+        <v>0.208596</v>
+      </c>
+      <c r="K5" s="62">
+        <v>9733</v>
+      </c>
+      <c r="L5" s="62">
+        <v>0.5</v>
+      </c>
+      <c r="M5" s="63"/>
+    </row>
+    <row r="6" spans="1:13" s="44" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A6" s="64" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" s="64" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="65" t="s">
+        <v>70</v>
+      </c>
+      <c r="D6" s="65" t="s">
+        <v>71</v>
+      </c>
+      <c r="E6" s="65" t="s">
+        <v>72</v>
+      </c>
+      <c r="F6" s="66" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="67" t="s">
+        <v>70</v>
+      </c>
+      <c r="H6" s="68">
+        <v>-6.3960000000000003E-2</v>
+      </c>
+      <c r="I6" s="68">
+        <v>-0.18359</v>
+      </c>
+      <c r="J6" s="68">
+        <v>5.9740000000000001E-2</v>
+      </c>
+      <c r="K6" s="68">
+        <v>9000</v>
+      </c>
+      <c r="L6" s="68">
+        <v>0.29899999999999999</v>
+      </c>
+      <c r="M6" s="69"/>
+    </row>
+    <row r="7" spans="1:13" s="44" customFormat="1" ht="15">
+      <c r="B7" s="46"/>
+      <c r="C7" s="46"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="45"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="43"/>
+      <c r="J7" s="43"/>
+      <c r="K7" s="43"/>
+      <c r="L7" s="43"/>
+      <c r="M7" s="43"/>
+    </row>
+    <row r="8" spans="1:13" s="44" customFormat="1" ht="15.75" thickBot="1">
+      <c r="B8" s="46"/>
+      <c r="C8" s="46"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="43"/>
+      <c r="I8" s="43"/>
+      <c r="J8" s="43"/>
+      <c r="K8" s="43"/>
+      <c r="L8" s="43"/>
+      <c r="M8" s="43"/>
+    </row>
+    <row r="9" spans="1:13" ht="21" customHeight="1" thickBot="1">
+      <c r="A9" s="71" t="s">
+        <v>80</v>
+      </c>
+      <c r="B9" s="72"/>
+      <c r="C9" s="72"/>
+      <c r="D9" s="72"/>
+      <c r="E9" s="72"/>
+      <c r="F9" s="72"/>
+      <c r="G9" s="72"/>
+      <c r="H9" s="72"/>
+      <c r="I9" s="72"/>
+      <c r="J9" s="72"/>
+      <c r="K9" s="72"/>
+      <c r="L9" s="72"/>
+      <c r="M9" s="73"/>
+    </row>
+    <row r="10" spans="1:13" s="42" customFormat="1" ht="16.5" thickBot="1">
+      <c r="A10" s="39" t="s">
+        <v>78</v>
+      </c>
+      <c r="B10" s="39" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="H10" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="I10" s="40" t="s">
+        <v>36</v>
+      </c>
+      <c r="J10" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="K10" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="L10" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="M10" s="41" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A11" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="H11" s="5">
+        <v>-0.15126000000000001</v>
+      </c>
+      <c r="I11" s="5">
+        <v>-0.35354000000000002</v>
+      </c>
+      <c r="J11" s="5">
+        <v>5.5750000000000001E-2</v>
+      </c>
+      <c r="K11" s="5">
+        <v>9000</v>
+      </c>
+      <c r="L11" s="5">
+        <v>0.158</v>
+      </c>
+      <c r="M11" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A12" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="37"/>
+      <c r="D12" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="H12" s="70">
+        <v>-3.7760000000000002E-2</v>
+      </c>
+      <c r="I12" s="70">
+        <v>-0.15218999999999999</v>
+      </c>
+      <c r="J12" s="70">
+        <v>8.6370000000000002E-2</v>
+      </c>
+      <c r="K12" s="70">
+        <v>9488</v>
+      </c>
+      <c r="L12" s="70">
+        <v>0.51600000000000001</v>
+      </c>
+      <c r="M12" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="74" t="s">
+        <v>82</v>
+      </c>
+      <c r="B13" s="76" t="s">
+        <v>84</v>
+      </c>
+      <c r="C13" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13" s="54" t="s">
+        <v>3</v>
+      </c>
+      <c r="H13" s="5">
+        <v>0.8256</v>
+      </c>
+      <c r="I13" s="5">
+        <v>-0.23598</v>
+      </c>
+      <c r="J13" s="5">
+        <v>1.8593900000000001</v>
+      </c>
+      <c r="K13" s="5">
+        <v>9346</v>
+      </c>
+      <c r="L13" s="5">
+        <v>0.103778</v>
+      </c>
+      <c r="M13" s="18"/>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" s="74"/>
+      <c r="B14" s="74"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="79" t="s">
+        <v>21</v>
+      </c>
+      <c r="H14" s="1">
+        <v>-2.1265700000000001</v>
+      </c>
+      <c r="I14" s="1">
+        <v>-2.3750200000000001</v>
+      </c>
+      <c r="J14" s="1">
+        <v>-1.87215</v>
+      </c>
+      <c r="K14" s="1">
+        <v>8588</v>
+      </c>
+      <c r="L14" s="78" t="s">
+        <v>85</v>
+      </c>
+      <c r="M14" s="86" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" s="74"/>
+      <c r="B15" s="74"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="50" t="s">
+        <v>47</v>
+      </c>
+      <c r="H15" s="1">
+        <v>-0.85921999999999998</v>
+      </c>
+      <c r="I15" s="1">
+        <v>-1.6769799999999999</v>
+      </c>
+      <c r="J15" s="1">
+        <v>5.3120000000000001E-2</v>
+      </c>
+      <c r="K15" s="1">
+        <v>8726</v>
+      </c>
+      <c r="L15" s="1">
+        <v>7.0444000000000007E-2</v>
+      </c>
+      <c r="M15" s="87" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="15" thickBot="1">
+      <c r="A16" s="75"/>
+      <c r="B16" s="74"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="80" t="s">
+        <v>48</v>
+      </c>
+      <c r="H16" s="7">
+        <v>-0.46776000000000001</v>
+      </c>
+      <c r="I16" s="7">
+        <v>-0.72677000000000003</v>
+      </c>
+      <c r="J16" s="7">
+        <v>-0.20458999999999999</v>
+      </c>
+      <c r="K16" s="7">
+        <v>9000</v>
+      </c>
+      <c r="L16" s="77">
+        <v>8.8900000000000003E-4</v>
+      </c>
+      <c r="M16" s="88" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" s="76" t="s">
+        <v>83</v>
+      </c>
+      <c r="B17" s="74"/>
+      <c r="C17" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="G17" s="54" t="s">
+        <v>3</v>
+      </c>
+      <c r="H17" s="82">
+        <v>0.79776499999999995</v>
+      </c>
+      <c r="I17" s="82">
+        <v>-0.64090599999999998</v>
+      </c>
+      <c r="J17" s="82">
+        <v>2.2084679999999999</v>
+      </c>
+      <c r="K17" s="82">
+        <v>8620</v>
+      </c>
+      <c r="L17" s="82">
+        <v>0.2127</v>
+      </c>
+      <c r="M17" s="83"/>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" s="74"/>
+      <c r="B18" s="74"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="79" t="s">
+        <v>21</v>
+      </c>
+      <c r="H18" s="81">
+        <v>-2.067698</v>
+      </c>
+      <c r="I18" s="81">
+        <v>-2.3194189999999999</v>
+      </c>
+      <c r="J18" s="81">
+        <v>-1.8245</v>
+      </c>
+      <c r="K18" s="81">
+        <v>9000</v>
+      </c>
+      <c r="L18" s="89" t="s">
+        <v>2</v>
+      </c>
+      <c r="M18" s="90" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" s="74"/>
+      <c r="B19" s="74"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="50" t="s">
+        <v>20</v>
+      </c>
+      <c r="H19" s="81">
+        <v>-0.238534</v>
+      </c>
+      <c r="I19" s="81">
+        <v>-1.070619</v>
+      </c>
+      <c r="J19" s="81">
+        <v>0.66691599999999995</v>
+      </c>
+      <c r="K19" s="81">
+        <v>7343</v>
+      </c>
+      <c r="L19" s="81">
+        <v>0.58779999999999999</v>
+      </c>
+      <c r="M19" s="84"/>
+    </row>
+    <row r="20" spans="1:13" ht="15" thickBot="1">
+      <c r="A20" s="75"/>
+      <c r="B20" s="75"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="37"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="37"/>
+      <c r="G20" s="93" t="s">
+        <v>19</v>
+      </c>
+      <c r="H20" s="70">
+        <v>-0.23789199999999999</v>
+      </c>
+      <c r="I20" s="70">
+        <v>-0.48010700000000001</v>
+      </c>
+      <c r="J20" s="70">
+        <v>7.8069999999999997E-3</v>
+      </c>
+      <c r="K20" s="70">
+        <v>9789</v>
+      </c>
+      <c r="L20" s="91">
+        <v>5.4899999999999997E-2</v>
+      </c>
+      <c r="M20" s="92" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A21" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="B21" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G21" s="94" t="s">
+        <v>16</v>
+      </c>
+      <c r="H21" s="5">
+        <v>-0.83430000000000004</v>
+      </c>
+      <c r="I21" s="5">
+        <v>-1.448</v>
+      </c>
+      <c r="J21" s="5">
+        <v>-0.1963</v>
+      </c>
+      <c r="K21" s="5">
+        <v>9000</v>
+      </c>
+      <c r="L21" s="94">
+        <v>1.8700000000000001E-2</v>
+      </c>
+      <c r="M21" s="100" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A22" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="B22" s="30"/>
+      <c r="C22" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H22" s="7">
+        <v>-0.84089999999999998</v>
+      </c>
+      <c r="I22" s="7">
+        <v>-2.5114999999999998</v>
+      </c>
+      <c r="J22" s="7">
+        <v>1.0492999999999999</v>
+      </c>
+      <c r="K22" s="7">
+        <v>9000</v>
+      </c>
+      <c r="L22" s="7">
+        <v>0.35299999999999998</v>
+      </c>
+      <c r="M22" s="19"/>
+    </row>
+    <row r="23" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A23" s="98" t="s">
+        <v>97</v>
+      </c>
+      <c r="B23" s="101" t="s">
+        <v>96</v>
+      </c>
+      <c r="C23" s="103" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="82" t="s">
+        <v>89</v>
+      </c>
+      <c r="E23" s="82" t="s">
+        <v>27</v>
+      </c>
+      <c r="F23" s="82" t="s">
+        <v>4</v>
+      </c>
+      <c r="G23" s="82" t="s">
+        <v>16</v>
+      </c>
+      <c r="H23" s="82">
+        <v>31.739000000000001</v>
+      </c>
+      <c r="I23" s="82">
+        <v>-9.5820000000000007</v>
+      </c>
+      <c r="J23" s="82">
+        <v>74.629000000000005</v>
+      </c>
+      <c r="K23" s="82">
+        <v>9293</v>
+      </c>
+      <c r="L23" s="82">
+        <v>0.12839999999999999</v>
+      </c>
+      <c r="M23" s="83"/>
+    </row>
+    <row r="24" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A24" s="99" t="s">
+        <v>98</v>
+      </c>
+      <c r="B24" s="102"/>
+      <c r="C24" s="104" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="70" t="s">
+        <v>92</v>
+      </c>
+      <c r="E24" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="F24" s="70" t="s">
+        <v>4</v>
+      </c>
+      <c r="G24" s="70" t="s">
+        <v>7</v>
+      </c>
+      <c r="H24" s="70">
+        <v>79.024000000000001</v>
+      </c>
+      <c r="I24" s="70">
+        <v>-15.327999999999999</v>
+      </c>
+      <c r="J24" s="70">
+        <v>178.03800000000001</v>
+      </c>
+      <c r="K24" s="70">
+        <v>9000</v>
+      </c>
+      <c r="L24" s="70">
+        <v>0.104</v>
+      </c>
+      <c r="M24" s="85" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A25" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="B25" s="95" t="s">
+        <v>90</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H25" s="5">
+        <v>0.219</v>
+      </c>
+      <c r="I25" s="5">
+        <v>-0.1174</v>
+      </c>
+      <c r="J25" s="5">
+        <v>0.58819999999999995</v>
+      </c>
+      <c r="K25" s="5">
+        <v>9000</v>
+      </c>
+      <c r="L25" s="5">
+        <v>0.20799999999999999</v>
+      </c>
+      <c r="M25" s="18"/>
+    </row>
+    <row r="26" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A26" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="B26" s="97"/>
+      <c r="C26" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H26" s="7">
+        <v>0.42120000000000002</v>
+      </c>
+      <c r="I26" s="7">
+        <v>-0.43430000000000002</v>
+      </c>
+      <c r="J26" s="7">
+        <v>1.1946000000000001</v>
+      </c>
+      <c r="K26" s="7">
+        <v>9000</v>
+      </c>
+      <c r="L26" s="7">
+        <v>0.29399999999999998</v>
+      </c>
+      <c r="M26" s="19"/>
+    </row>
+    <row r="27" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A27" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E27" s="96" t="s">
+        <v>27</v>
+      </c>
+      <c r="F27" s="96" t="s">
+        <v>4</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="H27" s="5">
+        <v>5.3220000000000003E-2</v>
+      </c>
+      <c r="I27" s="5">
+        <v>-0.62327999999999995</v>
+      </c>
+      <c r="J27" s="5">
+        <v>0.70852999999999999</v>
+      </c>
+      <c r="K27" s="5">
+        <v>9000</v>
+      </c>
+      <c r="L27" s="5">
+        <v>0.877</v>
+      </c>
+      <c r="M27" s="18"/>
+    </row>
+    <row r="28" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A28" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" s="37"/>
+      <c r="D28" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="H28" s="7">
+        <v>-0.1163</v>
+      </c>
+      <c r="I28" s="7">
+        <v>-0.44919999999999999</v>
+      </c>
+      <c r="J28" s="7">
+        <v>0.22589999999999999</v>
+      </c>
+      <c r="K28" s="7">
+        <v>9000</v>
+      </c>
+      <c r="L28" s="7">
+        <v>0.49199999999999999</v>
+      </c>
+      <c r="M28" s="19"/>
+    </row>
+    <row r="29" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A29" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="B29" s="107" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="D29" s="105" t="s">
+        <v>104</v>
+      </c>
+      <c r="E29" s="96" t="s">
+        <v>27</v>
+      </c>
+      <c r="F29" s="96" t="s">
+        <v>4</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H29" s="5">
+        <v>-1.961E-4</v>
+      </c>
+      <c r="I29" s="5">
+        <v>-6.1649999999999997E-4</v>
+      </c>
+      <c r="J29" s="5">
+        <v>1.8039999999999999E-4</v>
+      </c>
+      <c r="K29" s="5">
+        <v>9352</v>
+      </c>
+      <c r="L29" s="5">
+        <v>0.32200000000000001</v>
+      </c>
+      <c r="M29" s="18"/>
+    </row>
+    <row r="30" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A30" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="B30" s="106" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" s="37"/>
+      <c r="D30" s="106" t="s">
+        <v>105</v>
+      </c>
+      <c r="E30" s="106" t="s">
+        <v>5</v>
+      </c>
+      <c r="F30" s="106" t="s">
+        <v>4</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H30" s="7">
+        <v>-7.1400000000000001E-5</v>
+      </c>
+      <c r="I30" s="7">
+        <v>-3.0219999999999997E-4</v>
+      </c>
+      <c r="J30" s="7">
+        <v>1.7019999999999999E-4</v>
+      </c>
+      <c r="K30" s="7">
+        <v>9000</v>
+      </c>
+      <c r="L30" s="7">
+        <v>0.54200000000000004</v>
+      </c>
+      <c r="M30" s="19"/>
+    </row>
+    <row r="31" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A31" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="B31" s="105" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="D31" s="105" t="s">
+        <v>110</v>
+      </c>
+      <c r="E31" s="105" t="s">
+        <v>5</v>
+      </c>
+      <c r="F31" s="105" t="s">
+        <v>4</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H31" s="5">
+        <v>2.1640000000000001E-3</v>
+      </c>
+      <c r="I31" s="5">
+        <v>-4.594E-3</v>
+      </c>
+      <c r="J31" s="5">
+        <v>8.4709999999999994E-3</v>
+      </c>
+      <c r="K31" s="5">
+        <v>9000</v>
+      </c>
+      <c r="L31" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="M31" s="18"/>
+    </row>
+    <row r="32" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A32" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="B32" s="106" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" s="37"/>
+      <c r="D32" s="106" t="s">
+        <v>111</v>
+      </c>
+      <c r="E32" s="106" t="s">
+        <v>5</v>
+      </c>
+      <c r="F32" s="106" t="s">
+        <v>4</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="H32" s="7">
+        <v>7.4509999999999995E-4</v>
+      </c>
+      <c r="I32" s="7">
+        <v>-3.0501E-3</v>
+      </c>
+      <c r="J32" s="7">
+        <v>4.5215999999999998E-3</v>
+      </c>
+      <c r="K32" s="7">
+        <v>9000</v>
+      </c>
+      <c r="L32" s="7">
+        <v>0.68200000000000005</v>
+      </c>
+      <c r="M32" s="19"/>
+    </row>
+  </sheetData>
+  <mergeCells count="26">
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A9:M9"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="A13:A16"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="F3:F5"/>
+    <mergeCell ref="E3:E5"/>
+    <mergeCell ref="D3:D5"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="B13:B20"/>
+    <mergeCell ref="C13:C16"/>
+    <mergeCell ref="D13:D16"/>
+    <mergeCell ref="E13:E16"/>
+    <mergeCell ref="F13:F16"/>
+    <mergeCell ref="C17:C20"/>
+    <mergeCell ref="D17:D20"/>
+    <mergeCell ref="E17:E20"/>
+    <mergeCell ref="F17:F20"/>
+  </mergeCells>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="51" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="68.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="68.875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10.75" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="12" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" s="12" customFormat="1" ht="18.75" thickBot="1">
       <c r="A1" s="15" t="s">
         <v>43</v>
       </c>
@@ -992,11 +2643,11 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13">
       <c r="A2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="34" t="s">
         <v>44</v>
       </c>
       <c r="C2" s="5" t="s">
@@ -1033,11 +2684,11 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="15" thickBot="1">
       <c r="A3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="28"/>
+      <c r="B3" s="37"/>
       <c r="C3" s="7" t="s">
         <v>30</v>
       </c>
@@ -1072,20 +2723,20 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="29" t="s">
+    <row r="4" spans="1:13">
+      <c r="A4" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="30" t="s">
+      <c r="E4" s="36" t="s">
         <v>24</v>
       </c>
       <c r="F4" s="6" t="s">
@@ -1113,12 +2764,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="29"/>
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
+    <row r="5" spans="1:13">
+      <c r="A5" s="38"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
       <c r="F5" s="2" t="s">
         <v>21</v>
       </c>
@@ -1142,12 +2793,12 @@
       </c>
       <c r="M5" s="32"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="29"/>
-      <c r="B6" s="31"/>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
+    <row r="6" spans="1:13">
+      <c r="A6" s="38"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
       <c r="F6" s="2" t="s">
         <v>47</v>
       </c>
@@ -1169,12 +2820,12 @@
       <c r="L6" s="1"/>
       <c r="M6" s="32"/>
     </row>
-    <row r="7" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="29"/>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
+    <row r="7" spans="1:13" ht="15" thickBot="1">
+      <c r="A7" s="38"/>
+      <c r="B7" s="37"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
       <c r="F7" s="23" t="s">
         <v>48</v>
       </c>
@@ -1196,20 +2847,20 @@
       <c r="L7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="M7" s="30"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="29"/>
-      <c r="B8" s="27" t="s">
+      <c r="M7" s="36"/>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" s="38"/>
+      <c r="B8" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="27" t="s">
+      <c r="D8" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="27" t="s">
+      <c r="E8" s="34" t="s">
         <v>24</v>
       </c>
       <c r="F8" s="6" t="s">
@@ -1237,12 +2888,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="29"/>
-      <c r="B9" s="31"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
+    <row r="9" spans="1:13">
+      <c r="A9" s="38"/>
+      <c r="B9" s="35"/>
+      <c r="C9" s="35"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="35"/>
       <c r="F9" s="2" t="s">
         <v>21</v>
       </c>
@@ -1266,12 +2917,12 @@
       </c>
       <c r="M9" s="32"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="29"/>
-      <c r="B10" s="31"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
+    <row r="10" spans="1:13">
+      <c r="A10" s="38"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
       <c r="F10" s="2" t="s">
         <v>23</v>
       </c>
@@ -1293,12 +2944,12 @@
       <c r="L10" s="1"/>
       <c r="M10" s="32"/>
     </row>
-    <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="29"/>
-      <c r="B11" s="28"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
+    <row r="11" spans="1:13" ht="15" thickBot="1">
+      <c r="A11" s="38"/>
+      <c r="B11" s="37"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
       <c r="F11" s="23" t="s">
         <v>22</v>
       </c>
@@ -1318,20 +2969,20 @@
         <v>0.15329999999999999</v>
       </c>
       <c r="L11" s="26"/>
-      <c r="M11" s="30"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="29"/>
-      <c r="B12" s="27" t="s">
+      <c r="M11" s="36"/>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="38"/>
+      <c r="B12" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="27" t="s">
+      <c r="C12" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="27" t="s">
+      <c r="D12" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="27" t="s">
+      <c r="E12" s="34" t="s">
         <v>24</v>
       </c>
       <c r="F12" s="6" t="s">
@@ -1359,12 +3010,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="29"/>
-      <c r="B13" s="31"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
+    <row r="13" spans="1:13">
+      <c r="A13" s="38"/>
+      <c r="B13" s="35"/>
+      <c r="C13" s="35"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="35"/>
       <c r="F13" s="2" t="s">
         <v>21</v>
       </c>
@@ -1388,12 +3039,12 @@
       </c>
       <c r="M13" s="32"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="29"/>
-      <c r="B14" s="31"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
+    <row r="14" spans="1:13">
+      <c r="A14" s="38"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
       <c r="F14" s="2" t="s">
         <v>20</v>
       </c>
@@ -1415,8 +3066,8 @@
       <c r="L14" s="1"/>
       <c r="M14" s="32"/>
     </row>
-    <row r="15" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="29"/>
+    <row r="15" spans="1:13" ht="15" thickBot="1">
+      <c r="A15" s="38"/>
       <c r="B15" s="33"/>
       <c r="C15" s="33"/>
       <c r="D15" s="33"/>
@@ -1442,8 +3093,8 @@
       <c r="L15" s="26"/>
       <c r="M15" s="32"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="34" t="s">
+    <row r="16" spans="1:13">
+      <c r="A16" s="29" t="s">
         <v>52</v>
       </c>
       <c r="B16" s="5" t="s">
@@ -1483,8 +3134,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="35"/>
+    <row r="17" spans="1:13" ht="15" thickBot="1">
+      <c r="A17" s="30"/>
       <c r="B17" s="7" t="s">
         <v>14</v>
       </c>
@@ -1520,8 +3171,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="34" t="s">
+    <row r="18" spans="1:13">
+      <c r="A18" s="29" t="s">
         <v>18</v>
       </c>
       <c r="B18" s="5" t="s">
@@ -1559,8 +3210,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="36"/>
+    <row r="19" spans="1:13" ht="15" thickBot="1">
+      <c r="A19" s="31"/>
       <c r="B19" s="7" t="s">
         <v>14</v>
       </c>
@@ -1598,8 +3249,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="36"/>
+    <row r="20" spans="1:13">
+      <c r="A20" s="31"/>
       <c r="B20" s="5" t="s">
         <v>16</v>
       </c>
@@ -1633,8 +3284,8 @@
       <c r="L20" s="5"/>
       <c r="M20" s="18"/>
     </row>
-    <row r="21" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="36"/>
+    <row r="21" spans="1:13" ht="15" thickBot="1">
+      <c r="A21" s="31"/>
       <c r="B21" s="7" t="s">
         <v>14</v>
       </c>
@@ -1668,8 +3319,8 @@
       <c r="L21" s="7"/>
       <c r="M21" s="19"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="36"/>
+    <row r="22" spans="1:13">
+      <c r="A22" s="31"/>
       <c r="B22" s="5" t="s">
         <v>16</v>
       </c>
@@ -1703,8 +3354,8 @@
       <c r="L22" s="5"/>
       <c r="M22" s="18"/>
     </row>
-    <row r="23" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="35"/>
+    <row r="23" spans="1:13" ht="15" thickBot="1">
+      <c r="A23" s="30"/>
       <c r="B23" s="7" t="s">
         <v>14</v>
       </c>
@@ -1742,7 +3393,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" ht="15" thickBot="1">
       <c r="A24" s="9" t="s">
         <v>16</v>
       </c>
@@ -1781,7 +3432,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" ht="15" thickBot="1">
       <c r="A25" s="1" t="s">
         <v>14</v>
       </c>
@@ -1818,7 +3469,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" ht="15" thickBot="1">
       <c r="A26" s="1" t="s">
         <v>16</v>
       </c>
@@ -1845,11 +3496,11 @@
       <c r="L26" s="1"/>
       <c r="M26" s="4"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13">
       <c r="A27" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B27" s="30"/>
+      <c r="B27" s="36"/>
       <c r="C27" s="3" t="s">
         <v>6</v>
       </c>
@@ -1870,7 +3521,7 @@
       <c r="L27" s="1"/>
       <c r="M27" s="3"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13">
       <c r="A28" s="3" t="s">
         <v>8</v>
       </c>
@@ -1897,7 +3548,7 @@
       <c r="L28" s="1"/>
       <c r="M28" s="22"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13">
       <c r="A29" s="3" t="s">
         <v>7</v>
       </c>
@@ -1924,12 +3575,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A18:A23"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="B26:B27"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="A4:A15"/>
     <mergeCell ref="B4:B7"/>
@@ -1946,6 +3591,12 @@
     <mergeCell ref="C12:C15"/>
     <mergeCell ref="D12:D15"/>
     <mergeCell ref="E12:E15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A18:A23"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="B26:B27"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="51" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Snow model results added
</commit_message>
<xml_diff>
--- a/results/MCMC_model results .xlsx
+++ b/results/MCMC_model results .xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="118">
   <si>
     <t>FDD</t>
   </si>
@@ -375,6 +375,21 @@
   </si>
   <si>
     <t>Lratio ~ ecology</t>
+  </si>
+  <si>
+    <t>g17</t>
+  </si>
+  <si>
+    <t>g18</t>
+  </si>
+  <si>
+    <t>Snow</t>
+  </si>
+  <si>
+    <t>Loil.content ~ Snow</t>
+  </si>
+  <si>
+    <t>Lratio  ~ Snow</t>
   </si>
 </sst>
 </file>
@@ -891,7 +906,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -951,30 +966,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
@@ -991,34 +982,16 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1039,24 +1012,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1081,13 +1036,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1095,12 +1044,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1111,6 +1054,84 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1453,10 +1474,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M32"/>
+  <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -1476,280 +1497,280 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="21" customHeight="1" thickBot="1">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="84" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
-      <c r="H1" s="72"/>
-      <c r="I1" s="72"/>
-      <c r="J1" s="72"/>
-      <c r="K1" s="72"/>
-      <c r="L1" s="72"/>
-      <c r="M1" s="73"/>
-    </row>
-    <row r="2" spans="1:13" s="42" customFormat="1" ht="16.5" thickBot="1">
-      <c r="A2" s="39" t="s">
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="85"/>
+      <c r="H1" s="85"/>
+      <c r="I1" s="85"/>
+      <c r="J1" s="85"/>
+      <c r="K1" s="85"/>
+      <c r="L1" s="85"/>
+      <c r="M1" s="86"/>
+    </row>
+    <row r="2" spans="1:13" s="34" customFormat="1" ht="16.5" thickBot="1">
+      <c r="A2" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="40" t="s">
+      <c r="C2" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="40" t="s">
+      <c r="D2" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="E2" s="40" t="s">
+      <c r="E2" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="F2" s="40" t="s">
+      <c r="F2" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="G2" s="40" t="s">
+      <c r="G2" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="H2" s="40" t="s">
+      <c r="H2" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="I2" s="40" t="s">
+      <c r="I2" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="J2" s="40" t="s">
+      <c r="J2" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="K2" s="40" t="s">
+      <c r="K2" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="L2" s="40" t="s">
+      <c r="L2" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="M2" s="48" t="s">
+      <c r="M2" s="40" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="44" customFormat="1" ht="15">
-      <c r="A3" s="52" t="s">
+    <row r="3" spans="1:13" s="36" customFormat="1" ht="15">
+      <c r="A3" s="87" t="s">
         <v>74</v>
       </c>
-      <c r="B3" s="52" t="s">
+      <c r="B3" s="87" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="53" t="s">
+      <c r="C3" s="100" t="s">
         <v>65</v>
       </c>
-      <c r="D3" s="53" t="s">
+      <c r="D3" s="100" t="s">
         <v>66</v>
       </c>
-      <c r="E3" s="53" t="s">
+      <c r="E3" s="100" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="34" t="s">
+      <c r="F3" s="97" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="54" t="s">
+      <c r="G3" s="43" t="s">
         <v>69</v>
       </c>
-      <c r="H3" s="55">
+      <c r="H3" s="44">
         <v>2.1250909999999998</v>
       </c>
-      <c r="I3" s="55">
+      <c r="I3" s="44">
         <v>1.4455420000000001</v>
       </c>
-      <c r="J3" s="55">
+      <c r="J3" s="44">
         <v>2.8028209999999998</v>
       </c>
-      <c r="K3" s="55">
+      <c r="K3" s="44">
         <v>9000</v>
       </c>
-      <c r="L3" s="55" t="s">
+      <c r="L3" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="M3" s="56" t="s">
+      <c r="M3" s="45" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="44" customFormat="1" ht="15">
-      <c r="A4" s="57"/>
-      <c r="B4" s="57"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="50" t="s">
+    <row r="4" spans="1:13" s="36" customFormat="1" ht="15">
+      <c r="A4" s="88"/>
+      <c r="B4" s="88"/>
+      <c r="C4" s="101"/>
+      <c r="D4" s="101"/>
+      <c r="E4" s="101"/>
+      <c r="F4" s="98"/>
+      <c r="G4" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="H4" s="51">
+      <c r="H4" s="42">
         <v>-8.9210000000000001E-3</v>
       </c>
-      <c r="I4" s="51">
+      <c r="I4" s="42">
         <v>-0.28595799999999999</v>
       </c>
-      <c r="J4" s="51">
+      <c r="J4" s="42">
         <v>0.25387199999999999</v>
       </c>
-      <c r="K4" s="51">
+      <c r="K4" s="42">
         <v>8661</v>
       </c>
-      <c r="L4" s="51">
+      <c r="L4" s="42">
         <v>0.94699999999999995</v>
       </c>
-      <c r="M4" s="58"/>
-    </row>
-    <row r="5" spans="1:13" s="44" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A5" s="59"/>
-      <c r="B5" s="59"/>
-      <c r="C5" s="60"/>
-      <c r="D5" s="60"/>
-      <c r="E5" s="60"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="61" t="s">
+      <c r="M4" s="46"/>
+    </row>
+    <row r="5" spans="1:13" s="36" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A5" s="89"/>
+      <c r="B5" s="89"/>
+      <c r="C5" s="102"/>
+      <c r="D5" s="102"/>
+      <c r="E5" s="102"/>
+      <c r="F5" s="99"/>
+      <c r="G5" s="47" t="s">
         <v>68</v>
       </c>
-      <c r="H5" s="62">
+      <c r="H5" s="48">
         <v>-0.107848</v>
       </c>
-      <c r="I5" s="62">
+      <c r="I5" s="48">
         <v>-0.41161500000000001</v>
       </c>
-      <c r="J5" s="62">
+      <c r="J5" s="48">
         <v>0.208596</v>
       </c>
-      <c r="K5" s="62">
+      <c r="K5" s="48">
         <v>9733</v>
       </c>
-      <c r="L5" s="62">
+      <c r="L5" s="48">
         <v>0.5</v>
       </c>
-      <c r="M5" s="63"/>
-    </row>
-    <row r="6" spans="1:13" s="44" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A6" s="64" t="s">
+      <c r="M5" s="49"/>
+    </row>
+    <row r="6" spans="1:13" s="36" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A6" s="50" t="s">
         <v>75</v>
       </c>
-      <c r="B6" s="64" t="s">
+      <c r="B6" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="65" t="s">
+      <c r="C6" s="51" t="s">
         <v>70</v>
       </c>
-      <c r="D6" s="65" t="s">
+      <c r="D6" s="51" t="s">
         <v>71</v>
       </c>
-      <c r="E6" s="65" t="s">
+      <c r="E6" s="51" t="s">
         <v>72</v>
       </c>
-      <c r="F6" s="66" t="s">
+      <c r="F6" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="67" t="s">
+      <c r="G6" s="53" t="s">
         <v>70</v>
       </c>
-      <c r="H6" s="68">
+      <c r="H6" s="54">
         <v>-6.3960000000000003E-2</v>
       </c>
-      <c r="I6" s="68">
+      <c r="I6" s="54">
         <v>-0.18359</v>
       </c>
-      <c r="J6" s="68">
+      <c r="J6" s="54">
         <v>5.9740000000000001E-2</v>
       </c>
-      <c r="K6" s="68">
+      <c r="K6" s="54">
         <v>9000</v>
       </c>
-      <c r="L6" s="68">
+      <c r="L6" s="54">
         <v>0.29899999999999999</v>
       </c>
-      <c r="M6" s="69"/>
-    </row>
-    <row r="7" spans="1:13" s="44" customFormat="1" ht="15">
-      <c r="B7" s="46"/>
-      <c r="C7" s="46"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="47"/>
-      <c r="G7" s="45"/>
-      <c r="H7" s="43"/>
-      <c r="I7" s="43"/>
-      <c r="J7" s="43"/>
-      <c r="K7" s="43"/>
-      <c r="L7" s="43"/>
-      <c r="M7" s="43"/>
-    </row>
-    <row r="8" spans="1:13" s="44" customFormat="1" ht="15.75" thickBot="1">
-      <c r="B8" s="46"/>
-      <c r="C8" s="46"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="47"/>
-      <c r="G8" s="45"/>
-      <c r="H8" s="43"/>
-      <c r="I8" s="43"/>
-      <c r="J8" s="43"/>
-      <c r="K8" s="43"/>
-      <c r="L8" s="43"/>
-      <c r="M8" s="43"/>
+      <c r="M6" s="55"/>
+    </row>
+    <row r="7" spans="1:13" s="36" customFormat="1" ht="15">
+      <c r="B7" s="38"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="35"/>
+      <c r="I7" s="35"/>
+      <c r="J7" s="35"/>
+      <c r="K7" s="35"/>
+      <c r="L7" s="35"/>
+      <c r="M7" s="35"/>
+    </row>
+    <row r="8" spans="1:13" s="36" customFormat="1" ht="15.75" thickBot="1">
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="35"/>
+      <c r="I8" s="35"/>
+      <c r="J8" s="35"/>
+      <c r="K8" s="35"/>
+      <c r="L8" s="35"/>
+      <c r="M8" s="35"/>
     </row>
     <row r="9" spans="1:13" ht="21" customHeight="1" thickBot="1">
-      <c r="A9" s="71" t="s">
+      <c r="A9" s="84" t="s">
         <v>80</v>
       </c>
-      <c r="B9" s="72"/>
-      <c r="C9" s="72"/>
-      <c r="D9" s="72"/>
-      <c r="E9" s="72"/>
-      <c r="F9" s="72"/>
-      <c r="G9" s="72"/>
-      <c r="H9" s="72"/>
-      <c r="I9" s="72"/>
-      <c r="J9" s="72"/>
-      <c r="K9" s="72"/>
-      <c r="L9" s="72"/>
-      <c r="M9" s="73"/>
-    </row>
-    <row r="10" spans="1:13" s="42" customFormat="1" ht="16.5" thickBot="1">
-      <c r="A10" s="39" t="s">
+      <c r="B9" s="85"/>
+      <c r="C9" s="85"/>
+      <c r="D9" s="85"/>
+      <c r="E9" s="85"/>
+      <c r="F9" s="85"/>
+      <c r="G9" s="85"/>
+      <c r="H9" s="85"/>
+      <c r="I9" s="85"/>
+      <c r="J9" s="85"/>
+      <c r="K9" s="85"/>
+      <c r="L9" s="85"/>
+      <c r="M9" s="86"/>
+    </row>
+    <row r="10" spans="1:13" s="34" customFormat="1" ht="16.5" thickBot="1">
+      <c r="A10" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="B10" s="39" t="s">
+      <c r="B10" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="C10" s="40" t="s">
+      <c r="C10" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="40" t="s">
+      <c r="D10" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="E10" s="40" t="s">
+      <c r="E10" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="F10" s="40" t="s">
+      <c r="F10" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="G10" s="40" t="s">
+      <c r="G10" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="H10" s="40" t="s">
+      <c r="H10" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="I10" s="40" t="s">
+      <c r="I10" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="J10" s="40" t="s">
+      <c r="J10" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="K10" s="40" t="s">
+      <c r="K10" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="L10" s="40" t="s">
+      <c r="L10" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="M10" s="41" t="s">
+      <c r="M10" s="33" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1760,7 +1781,7 @@
       <c r="B11" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="34" t="s">
+      <c r="C11" s="97" t="s">
         <v>79</v>
       </c>
       <c r="D11" s="5" t="s">
@@ -1801,7 +1822,7 @@
       <c r="B12" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="37"/>
+      <c r="C12" s="99"/>
       <c r="D12" s="7" t="s">
         <v>95</v>
       </c>
@@ -1814,19 +1835,19 @@
       <c r="G12" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="H12" s="70">
+      <c r="H12" s="56">
         <v>-3.7760000000000002E-2</v>
       </c>
-      <c r="I12" s="70">
+      <c r="I12" s="56">
         <v>-0.15218999999999999</v>
       </c>
-      <c r="J12" s="70">
+      <c r="J12" s="56">
         <v>8.6370000000000002E-2</v>
       </c>
-      <c r="K12" s="70">
+      <c r="K12" s="56">
         <v>9488</v>
       </c>
-      <c r="L12" s="70">
+      <c r="L12" s="56">
         <v>0.51600000000000001</v>
       </c>
       <c r="M12" s="7" t="s">
@@ -1834,25 +1855,25 @@
       </c>
     </row>
     <row r="13" spans="1:13">
-      <c r="A13" s="74" t="s">
+      <c r="A13" s="91" t="s">
         <v>82</v>
       </c>
-      <c r="B13" s="76" t="s">
+      <c r="B13" s="90" t="s">
         <v>84</v>
       </c>
-      <c r="C13" s="29" t="s">
+      <c r="C13" s="103" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="34" t="s">
+      <c r="D13" s="97" t="s">
         <v>46</v>
       </c>
-      <c r="E13" s="34" t="s">
+      <c r="E13" s="97" t="s">
         <v>27</v>
       </c>
-      <c r="F13" s="34" t="s">
+      <c r="F13" s="97" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="54" t="s">
+      <c r="G13" s="43" t="s">
         <v>3</v>
       </c>
       <c r="H13" s="5">
@@ -1873,13 +1894,13 @@
       <c r="M13" s="18"/>
     </row>
     <row r="14" spans="1:13">
-      <c r="A14" s="74"/>
-      <c r="B14" s="74"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="35"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="79" t="s">
+      <c r="A14" s="91"/>
+      <c r="B14" s="91"/>
+      <c r="C14" s="105"/>
+      <c r="D14" s="98"/>
+      <c r="E14" s="98"/>
+      <c r="F14" s="98"/>
+      <c r="G14" s="59" t="s">
         <v>21</v>
       </c>
       <c r="H14" s="1">
@@ -1894,21 +1915,21 @@
       <c r="K14" s="1">
         <v>8588</v>
       </c>
-      <c r="L14" s="78" t="s">
+      <c r="L14" s="58" t="s">
         <v>85</v>
       </c>
-      <c r="M14" s="86" t="s">
+      <c r="M14" s="66" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:13">
-      <c r="A15" s="74"/>
-      <c r="B15" s="74"/>
-      <c r="C15" s="31"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35"/>
-      <c r="G15" s="50" t="s">
+      <c r="A15" s="91"/>
+      <c r="B15" s="91"/>
+      <c r="C15" s="105"/>
+      <c r="D15" s="98"/>
+      <c r="E15" s="98"/>
+      <c r="F15" s="98"/>
+      <c r="G15" s="41" t="s">
         <v>47</v>
       </c>
       <c r="H15" s="1">
@@ -1926,18 +1947,18 @@
       <c r="L15" s="1">
         <v>7.0444000000000007E-2</v>
       </c>
-      <c r="M15" s="87" t="s">
+      <c r="M15" s="67" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="15" thickBot="1">
-      <c r="A16" s="75"/>
-      <c r="B16" s="74"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="80" t="s">
+      <c r="A16" s="92"/>
+      <c r="B16" s="91"/>
+      <c r="C16" s="104"/>
+      <c r="D16" s="99"/>
+      <c r="E16" s="99"/>
+      <c r="F16" s="99"/>
+      <c r="G16" s="60" t="s">
         <v>48</v>
       </c>
       <c r="H16" s="7">
@@ -1952,132 +1973,132 @@
       <c r="K16" s="7">
         <v>9000</v>
       </c>
-      <c r="L16" s="77">
+      <c r="L16" s="57">
         <v>8.8900000000000003E-4</v>
       </c>
-      <c r="M16" s="88" t="s">
+      <c r="M16" s="68" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:13">
-      <c r="A17" s="76" t="s">
+      <c r="A17" s="90" t="s">
         <v>83</v>
       </c>
-      <c r="B17" s="74"/>
-      <c r="C17" s="29" t="s">
+      <c r="B17" s="91"/>
+      <c r="C17" s="103" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="34" t="s">
+      <c r="D17" s="97" t="s">
         <v>25</v>
       </c>
-      <c r="E17" s="34" t="s">
+      <c r="E17" s="97" t="s">
         <v>5</v>
       </c>
-      <c r="F17" s="34" t="s">
+      <c r="F17" s="97" t="s">
         <v>24</v>
       </c>
-      <c r="G17" s="54" t="s">
+      <c r="G17" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="H17" s="82">
+      <c r="H17" s="62">
         <v>0.79776499999999995</v>
       </c>
-      <c r="I17" s="82">
+      <c r="I17" s="62">
         <v>-0.64090599999999998</v>
       </c>
-      <c r="J17" s="82">
+      <c r="J17" s="62">
         <v>2.2084679999999999</v>
       </c>
-      <c r="K17" s="82">
+      <c r="K17" s="62">
         <v>8620</v>
       </c>
-      <c r="L17" s="82">
+      <c r="L17" s="62">
         <v>0.2127</v>
       </c>
-      <c r="M17" s="83"/>
+      <c r="M17" s="63"/>
     </row>
     <row r="18" spans="1:13">
-      <c r="A18" s="74"/>
-      <c r="B18" s="74"/>
-      <c r="C18" s="31"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="79" t="s">
+      <c r="A18" s="91"/>
+      <c r="B18" s="91"/>
+      <c r="C18" s="105"/>
+      <c r="D18" s="98"/>
+      <c r="E18" s="98"/>
+      <c r="F18" s="98"/>
+      <c r="G18" s="59" t="s">
         <v>21</v>
       </c>
-      <c r="H18" s="81">
+      <c r="H18" s="61">
         <v>-2.067698</v>
       </c>
-      <c r="I18" s="81">
+      <c r="I18" s="61">
         <v>-2.3194189999999999</v>
       </c>
-      <c r="J18" s="81">
+      <c r="J18" s="61">
         <v>-1.8245</v>
       </c>
-      <c r="K18" s="81">
+      <c r="K18" s="61">
         <v>9000</v>
       </c>
-      <c r="L18" s="89" t="s">
+      <c r="L18" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="M18" s="90" t="s">
+      <c r="M18" s="70" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:13">
-      <c r="A19" s="74"/>
-      <c r="B19" s="74"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="35"/>
-      <c r="F19" s="35"/>
-      <c r="G19" s="50" t="s">
+      <c r="A19" s="91"/>
+      <c r="B19" s="91"/>
+      <c r="C19" s="105"/>
+      <c r="D19" s="98"/>
+      <c r="E19" s="98"/>
+      <c r="F19" s="98"/>
+      <c r="G19" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="H19" s="81">
+      <c r="H19" s="61">
         <v>-0.238534</v>
       </c>
-      <c r="I19" s="81">
+      <c r="I19" s="61">
         <v>-1.070619</v>
       </c>
-      <c r="J19" s="81">
+      <c r="J19" s="61">
         <v>0.66691599999999995</v>
       </c>
-      <c r="K19" s="81">
+      <c r="K19" s="61">
         <v>7343</v>
       </c>
-      <c r="L19" s="81">
+      <c r="L19" s="61">
         <v>0.58779999999999999</v>
       </c>
-      <c r="M19" s="84"/>
+      <c r="M19" s="64"/>
     </row>
     <row r="20" spans="1:13" ht="15" thickBot="1">
-      <c r="A20" s="75"/>
-      <c r="B20" s="75"/>
-      <c r="C20" s="30"/>
-      <c r="D20" s="37"/>
-      <c r="E20" s="37"/>
-      <c r="F20" s="37"/>
-      <c r="G20" s="93" t="s">
+      <c r="A20" s="92"/>
+      <c r="B20" s="92"/>
+      <c r="C20" s="104"/>
+      <c r="D20" s="99"/>
+      <c r="E20" s="99"/>
+      <c r="F20" s="99"/>
+      <c r="G20" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="H20" s="70">
+      <c r="H20" s="56">
         <v>-0.23789199999999999</v>
       </c>
-      <c r="I20" s="70">
+      <c r="I20" s="56">
         <v>-0.48010700000000001</v>
       </c>
-      <c r="J20" s="70">
+      <c r="J20" s="56">
         <v>7.8069999999999997E-3</v>
       </c>
-      <c r="K20" s="70">
+      <c r="K20" s="56">
         <v>9789</v>
       </c>
-      <c r="L20" s="91">
+      <c r="L20" s="71">
         <v>5.4899999999999997E-2</v>
       </c>
-      <c r="M20" s="92" t="s">
+      <c r="M20" s="72" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2085,7 +2106,7 @@
       <c r="A21" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="B21" s="29" t="s">
+      <c r="B21" s="103" t="s">
         <v>88</v>
       </c>
       <c r="C21" s="5" t="s">
@@ -2100,7 +2121,7 @@
       <c r="F21" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G21" s="94" t="s">
+      <c r="G21" s="74" t="s">
         <v>16</v>
       </c>
       <c r="H21" s="5">
@@ -2115,10 +2136,10 @@
       <c r="K21" s="5">
         <v>9000</v>
       </c>
-      <c r="L21" s="94">
+      <c r="L21" s="74">
         <v>1.8700000000000001E-2</v>
       </c>
-      <c r="M21" s="100" t="s">
+      <c r="M21" s="78" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2126,7 +2147,7 @@
       <c r="A22" s="28" t="s">
         <v>87</v>
       </c>
-      <c r="B22" s="30"/>
+      <c r="B22" s="104"/>
       <c r="C22" s="7" t="s">
         <v>7</v>
       </c>
@@ -2160,80 +2181,80 @@
       <c r="M22" s="19"/>
     </row>
     <row r="23" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A23" s="98" t="s">
+      <c r="A23" s="76" t="s">
         <v>97</v>
       </c>
-      <c r="B23" s="101" t="s">
+      <c r="B23" s="95" t="s">
         <v>96</v>
       </c>
-      <c r="C23" s="103" t="s">
+      <c r="C23" s="79" t="s">
         <v>16</v>
       </c>
-      <c r="D23" s="82" t="s">
+      <c r="D23" s="62" t="s">
         <v>89</v>
       </c>
-      <c r="E23" s="82" t="s">
+      <c r="E23" s="62" t="s">
         <v>27</v>
       </c>
-      <c r="F23" s="82" t="s">
+      <c r="F23" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="G23" s="82" t="s">
+      <c r="G23" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="H23" s="82">
+      <c r="H23" s="62">
         <v>31.739000000000001</v>
       </c>
-      <c r="I23" s="82">
+      <c r="I23" s="62">
         <v>-9.5820000000000007</v>
       </c>
-      <c r="J23" s="82">
+      <c r="J23" s="62">
         <v>74.629000000000005</v>
       </c>
-      <c r="K23" s="82">
+      <c r="K23" s="62">
         <v>9293</v>
       </c>
-      <c r="L23" s="82">
+      <c r="L23" s="62">
         <v>0.12839999999999999</v>
       </c>
-      <c r="M23" s="83"/>
+      <c r="M23" s="63"/>
     </row>
     <row r="24" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A24" s="99" t="s">
+      <c r="A24" s="77" t="s">
         <v>98</v>
       </c>
-      <c r="B24" s="102"/>
-      <c r="C24" s="104" t="s">
+      <c r="B24" s="96"/>
+      <c r="C24" s="80" t="s">
         <v>7</v>
       </c>
-      <c r="D24" s="70" t="s">
+      <c r="D24" s="56" t="s">
         <v>92</v>
       </c>
-      <c r="E24" s="70" t="s">
+      <c r="E24" s="56" t="s">
         <v>27</v>
       </c>
-      <c r="F24" s="70" t="s">
+      <c r="F24" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="G24" s="70" t="s">
+      <c r="G24" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="H24" s="70">
+      <c r="H24" s="56">
         <v>79.024000000000001</v>
       </c>
-      <c r="I24" s="70">
+      <c r="I24" s="56">
         <v>-15.327999999999999</v>
       </c>
-      <c r="J24" s="70">
+      <c r="J24" s="56">
         <v>178.03800000000001</v>
       </c>
-      <c r="K24" s="70">
+      <c r="K24" s="56">
         <v>9000</v>
       </c>
-      <c r="L24" s="70">
+      <c r="L24" s="56">
         <v>0.104</v>
       </c>
-      <c r="M24" s="85" t="s">
+      <c r="M24" s="65" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2241,7 +2262,7 @@
       <c r="A25" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="B25" s="95" t="s">
+      <c r="B25" s="93" t="s">
         <v>90</v>
       </c>
       <c r="C25" s="5" t="s">
@@ -2280,7 +2301,7 @@
       <c r="A26" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="B26" s="97"/>
+      <c r="B26" s="94"/>
       <c r="C26" s="7" t="s">
         <v>7</v>
       </c>
@@ -2320,16 +2341,16 @@
       <c r="B27" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C27" s="34" t="s">
+      <c r="C27" s="97" t="s">
         <v>15</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="E27" s="96" t="s">
+      <c r="E27" s="75" t="s">
         <v>27</v>
       </c>
-      <c r="F27" s="96" t="s">
+      <c r="F27" s="75" t="s">
         <v>4</v>
       </c>
       <c r="G27" s="5" t="s">
@@ -2359,7 +2380,7 @@
       <c r="B28" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C28" s="37"/>
+      <c r="C28" s="99"/>
       <c r="D28" s="7" t="s">
         <v>112</v>
       </c>
@@ -2393,19 +2414,19 @@
       <c r="A29" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="B29" s="107" t="s">
+      <c r="B29" s="83" t="s">
         <v>16</v>
       </c>
-      <c r="C29" s="34" t="s">
+      <c r="C29" s="97" t="s">
         <v>9</v>
       </c>
-      <c r="D29" s="105" t="s">
+      <c r="D29" s="81" t="s">
         <v>104</v>
       </c>
-      <c r="E29" s="96" t="s">
+      <c r="E29" s="75" t="s">
         <v>27</v>
       </c>
-      <c r="F29" s="96" t="s">
+      <c r="F29" s="75" t="s">
         <v>4</v>
       </c>
       <c r="G29" s="5" t="s">
@@ -2432,17 +2453,17 @@
       <c r="A30" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="B30" s="106" t="s">
+      <c r="B30" s="82" t="s">
         <v>7</v>
       </c>
-      <c r="C30" s="37"/>
-      <c r="D30" s="106" t="s">
+      <c r="C30" s="99"/>
+      <c r="D30" s="82" t="s">
         <v>105</v>
       </c>
-      <c r="E30" s="106" t="s">
+      <c r="E30" s="82" t="s">
         <v>5</v>
       </c>
-      <c r="F30" s="106" t="s">
+      <c r="F30" s="82" t="s">
         <v>4</v>
       </c>
       <c r="G30" s="7" t="s">
@@ -2469,19 +2490,19 @@
       <c r="A31" s="27" t="s">
         <v>108</v>
       </c>
-      <c r="B31" s="105" t="s">
+      <c r="B31" s="81" t="s">
         <v>8</v>
       </c>
-      <c r="C31" s="34" t="s">
+      <c r="C31" s="97" t="s">
         <v>0</v>
       </c>
-      <c r="D31" s="105" t="s">
+      <c r="D31" s="81" t="s">
         <v>110</v>
       </c>
-      <c r="E31" s="105" t="s">
+      <c r="E31" s="81" t="s">
         <v>5</v>
       </c>
-      <c r="F31" s="105" t="s">
+      <c r="F31" s="81" t="s">
         <v>4</v>
       </c>
       <c r="G31" s="5" t="s">
@@ -2508,17 +2529,17 @@
       <c r="A32" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="B32" s="106" t="s">
+      <c r="B32" s="82" t="s">
         <v>7</v>
       </c>
-      <c r="C32" s="37"/>
-      <c r="D32" s="106" t="s">
+      <c r="C32" s="99"/>
+      <c r="D32" s="82" t="s">
         <v>111</v>
       </c>
-      <c r="E32" s="106" t="s">
+      <c r="E32" s="82" t="s">
         <v>5</v>
       </c>
-      <c r="F32" s="106" t="s">
+      <c r="F32" s="82" t="s">
         <v>4</v>
       </c>
       <c r="G32" s="7" t="s">
@@ -2541,13 +2562,94 @@
       </c>
       <c r="M32" s="19"/>
     </row>
+    <row r="33" spans="1:13">
+      <c r="A33" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="B33" s="81" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" s="97" t="s">
+        <v>115</v>
+      </c>
+      <c r="D33" s="81" t="s">
+        <v>116</v>
+      </c>
+      <c r="E33" s="81" t="s">
+        <v>5</v>
+      </c>
+      <c r="F33" s="81" t="s">
+        <v>4</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="H33" s="5">
+        <v>2.8960000000000001E-3</v>
+      </c>
+      <c r="I33" s="5">
+        <v>-1.4400000000000001E-3</v>
+      </c>
+      <c r="J33" s="5">
+        <v>7.1219999999999999E-3</v>
+      </c>
+      <c r="K33" s="5">
+        <v>9334</v>
+      </c>
+      <c r="L33" s="5">
+        <v>0.17399999999999999</v>
+      </c>
+      <c r="M33" s="18"/>
+    </row>
+    <row r="34" spans="1:13" ht="15" thickBot="1">
+      <c r="A34" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="B34" s="82" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" s="99"/>
+      <c r="D34" s="82" t="s">
+        <v>117</v>
+      </c>
+      <c r="E34" s="82" t="s">
+        <v>5</v>
+      </c>
+      <c r="F34" s="82" t="s">
+        <v>4</v>
+      </c>
+      <c r="G34" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="H34" s="7">
+        <v>2.0574E-3</v>
+      </c>
+      <c r="I34" s="7">
+        <v>-3.9639999999999999E-4</v>
+      </c>
+      <c r="J34" s="7">
+        <v>4.5411000000000002E-3</v>
+      </c>
+      <c r="K34" s="7">
+        <v>9323</v>
+      </c>
+      <c r="L34" s="7">
+        <v>9.5299999999999996E-2</v>
+      </c>
+      <c r="M34" s="19" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="26">
-    <mergeCell ref="A1:M1"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="A9:M9"/>
-    <mergeCell ref="A17:A20"/>
-    <mergeCell ref="A13:A16"/>
+  <mergeCells count="27">
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="B13:B20"/>
+    <mergeCell ref="C13:C16"/>
+    <mergeCell ref="C17:C20"/>
     <mergeCell ref="B25:B26"/>
     <mergeCell ref="B23:B24"/>
     <mergeCell ref="F3:F5"/>
@@ -2556,19 +2658,17 @@
     <mergeCell ref="C3:C5"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="B21:B22"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="B13:B20"/>
-    <mergeCell ref="C13:C16"/>
     <mergeCell ref="D13:D16"/>
     <mergeCell ref="E13:E16"/>
     <mergeCell ref="F13:F16"/>
-    <mergeCell ref="C17:C20"/>
     <mergeCell ref="D17:D20"/>
     <mergeCell ref="E17:E20"/>
     <mergeCell ref="F17:F20"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A9:M9"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="A13:A16"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="51" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -2647,7 +2747,7 @@
       <c r="A2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="97" t="s">
         <v>44</v>
       </c>
       <c r="C2" s="5" t="s">
@@ -2688,7 +2788,7 @@
       <c r="A3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="37"/>
+      <c r="B3" s="99"/>
       <c r="C3" s="7" t="s">
         <v>30</v>
       </c>
@@ -2724,19 +2824,19 @@
       </c>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="106" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="107" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="36" t="s">
+      <c r="C4" s="107" t="s">
         <v>46</v>
       </c>
-      <c r="D4" s="36" t="s">
+      <c r="D4" s="107" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="36" t="s">
+      <c r="E4" s="107" t="s">
         <v>24</v>
       </c>
       <c r="F4" s="6" t="s">
@@ -2760,16 +2860,16 @@
       <c r="L4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="32" t="s">
+      <c r="M4" s="108" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:13">
-      <c r="A5" s="38"/>
-      <c r="B5" s="35"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
+      <c r="A5" s="106"/>
+      <c r="B5" s="98"/>
+      <c r="C5" s="98"/>
+      <c r="D5" s="98"/>
+      <c r="E5" s="98"/>
       <c r="F5" s="2" t="s">
         <v>21</v>
       </c>
@@ -2791,14 +2891,14 @@
       <c r="L5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="M5" s="32"/>
+      <c r="M5" s="108"/>
     </row>
     <row r="6" spans="1:13">
-      <c r="A6" s="38"/>
-      <c r="B6" s="35"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
+      <c r="A6" s="106"/>
+      <c r="B6" s="98"/>
+      <c r="C6" s="98"/>
+      <c r="D6" s="98"/>
+      <c r="E6" s="98"/>
       <c r="F6" s="2" t="s">
         <v>47</v>
       </c>
@@ -2818,14 +2918,14 @@
         <v>0.28399999999999997</v>
       </c>
       <c r="L6" s="1"/>
-      <c r="M6" s="32"/>
+      <c r="M6" s="108"/>
     </row>
     <row r="7" spans="1:13" ht="15" thickBot="1">
-      <c r="A7" s="38"/>
-      <c r="B7" s="37"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
+      <c r="A7" s="106"/>
+      <c r="B7" s="99"/>
+      <c r="C7" s="99"/>
+      <c r="D7" s="99"/>
+      <c r="E7" s="99"/>
       <c r="F7" s="23" t="s">
         <v>48</v>
       </c>
@@ -2847,20 +2947,20 @@
       <c r="L7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="M7" s="36"/>
+      <c r="M7" s="107"/>
     </row>
     <row r="8" spans="1:13">
-      <c r="A8" s="38"/>
-      <c r="B8" s="34" t="s">
+      <c r="A8" s="106"/>
+      <c r="B8" s="97" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="34" t="s">
+      <c r="C8" s="97" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="34" t="s">
+      <c r="D8" s="97" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="34" t="s">
+      <c r="E8" s="97" t="s">
         <v>24</v>
       </c>
       <c r="F8" s="6" t="s">
@@ -2884,16 +2984,16 @@
       <c r="L8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="M8" s="33" t="s">
+      <c r="M8" s="109" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:13">
-      <c r="A9" s="38"/>
-      <c r="B9" s="35"/>
-      <c r="C9" s="35"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
+      <c r="A9" s="106"/>
+      <c r="B9" s="98"/>
+      <c r="C9" s="98"/>
+      <c r="D9" s="98"/>
+      <c r="E9" s="98"/>
       <c r="F9" s="2" t="s">
         <v>21</v>
       </c>
@@ -2915,14 +3015,14 @@
       <c r="L9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="M9" s="32"/>
+      <c r="M9" s="108"/>
     </row>
     <row r="10" spans="1:13">
-      <c r="A10" s="38"/>
-      <c r="B10" s="35"/>
-      <c r="C10" s="35"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="35"/>
+      <c r="A10" s="106"/>
+      <c r="B10" s="98"/>
+      <c r="C10" s="98"/>
+      <c r="D10" s="98"/>
+      <c r="E10" s="98"/>
       <c r="F10" s="2" t="s">
         <v>23</v>
       </c>
@@ -2942,14 +3042,14 @@
         <v>0.14799999999999999</v>
       </c>
       <c r="L10" s="1"/>
-      <c r="M10" s="32"/>
+      <c r="M10" s="108"/>
     </row>
     <row r="11" spans="1:13" ht="15" thickBot="1">
-      <c r="A11" s="38"/>
-      <c r="B11" s="37"/>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="37"/>
+      <c r="A11" s="106"/>
+      <c r="B11" s="99"/>
+      <c r="C11" s="99"/>
+      <c r="D11" s="99"/>
+      <c r="E11" s="99"/>
       <c r="F11" s="23" t="s">
         <v>22</v>
       </c>
@@ -2969,20 +3069,20 @@
         <v>0.15329999999999999</v>
       </c>
       <c r="L11" s="26"/>
-      <c r="M11" s="36"/>
+      <c r="M11" s="107"/>
     </row>
     <row r="12" spans="1:13">
-      <c r="A12" s="38"/>
-      <c r="B12" s="34" t="s">
+      <c r="A12" s="106"/>
+      <c r="B12" s="97" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="34" t="s">
+      <c r="C12" s="97" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="34" t="s">
+      <c r="D12" s="97" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="34" t="s">
+      <c r="E12" s="97" t="s">
         <v>24</v>
       </c>
       <c r="F12" s="6" t="s">
@@ -3006,16 +3106,16 @@
       <c r="L12" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="M12" s="33" t="s">
+      <c r="M12" s="109" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:13">
-      <c r="A13" s="38"/>
-      <c r="B13" s="35"/>
-      <c r="C13" s="35"/>
-      <c r="D13" s="35"/>
-      <c r="E13" s="35"/>
+      <c r="A13" s="106"/>
+      <c r="B13" s="98"/>
+      <c r="C13" s="98"/>
+      <c r="D13" s="98"/>
+      <c r="E13" s="98"/>
       <c r="F13" s="2" t="s">
         <v>21</v>
       </c>
@@ -3037,14 +3137,14 @@
       <c r="L13" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="M13" s="32"/>
+      <c r="M13" s="108"/>
     </row>
     <row r="14" spans="1:13">
-      <c r="A14" s="38"/>
-      <c r="B14" s="35"/>
-      <c r="C14" s="35"/>
-      <c r="D14" s="35"/>
-      <c r="E14" s="35"/>
+      <c r="A14" s="106"/>
+      <c r="B14" s="98"/>
+      <c r="C14" s="98"/>
+      <c r="D14" s="98"/>
+      <c r="E14" s="98"/>
       <c r="F14" s="2" t="s">
         <v>20</v>
       </c>
@@ -3064,14 +3164,14 @@
         <v>0.2258</v>
       </c>
       <c r="L14" s="1"/>
-      <c r="M14" s="32"/>
+      <c r="M14" s="108"/>
     </row>
     <row r="15" spans="1:13" ht="15" thickBot="1">
-      <c r="A15" s="38"/>
-      <c r="B15" s="33"/>
-      <c r="C15" s="33"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="33"/>
+      <c r="A15" s="106"/>
+      <c r="B15" s="109"/>
+      <c r="C15" s="109"/>
+      <c r="D15" s="109"/>
+      <c r="E15" s="109"/>
       <c r="F15" s="23" t="s">
         <v>19</v>
       </c>
@@ -3091,10 +3191,10 @@
         <v>0.22289999999999999</v>
       </c>
       <c r="L15" s="26"/>
-      <c r="M15" s="32"/>
+      <c r="M15" s="108"/>
     </row>
     <row r="16" spans="1:13">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="103" t="s">
         <v>52</v>
       </c>
       <c r="B16" s="5" t="s">
@@ -3135,7 +3235,7 @@
       </c>
     </row>
     <row r="17" spans="1:13" ht="15" thickBot="1">
-      <c r="A17" s="30"/>
+      <c r="A17" s="104"/>
       <c r="B17" s="7" t="s">
         <v>14</v>
       </c>
@@ -3172,7 +3272,7 @@
       </c>
     </row>
     <row r="18" spans="1:13">
-      <c r="A18" s="29" t="s">
+      <c r="A18" s="103" t="s">
         <v>18</v>
       </c>
       <c r="B18" s="5" t="s">
@@ -3211,7 +3311,7 @@
       </c>
     </row>
     <row r="19" spans="1:13" ht="15" thickBot="1">
-      <c r="A19" s="31"/>
+      <c r="A19" s="105"/>
       <c r="B19" s="7" t="s">
         <v>14</v>
       </c>
@@ -3250,7 +3350,7 @@
       </c>
     </row>
     <row r="20" spans="1:13">
-      <c r="A20" s="31"/>
+      <c r="A20" s="105"/>
       <c r="B20" s="5" t="s">
         <v>16</v>
       </c>
@@ -3285,7 +3385,7 @@
       <c r="M20" s="18"/>
     </row>
     <row r="21" spans="1:13" ht="15" thickBot="1">
-      <c r="A21" s="31"/>
+      <c r="A21" s="105"/>
       <c r="B21" s="7" t="s">
         <v>14</v>
       </c>
@@ -3320,7 +3420,7 @@
       <c r="M21" s="19"/>
     </row>
     <row r="22" spans="1:13">
-      <c r="A22" s="31"/>
+      <c r="A22" s="105"/>
       <c r="B22" s="5" t="s">
         <v>16</v>
       </c>
@@ -3355,7 +3455,7 @@
       <c r="M22" s="18"/>
     </row>
     <row r="23" spans="1:13" ht="15" thickBot="1">
-      <c r="A23" s="30"/>
+      <c r="A23" s="104"/>
       <c r="B23" s="7" t="s">
         <v>14</v>
       </c>
@@ -3397,7 +3497,7 @@
       <c r="A24" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B24" s="32" t="s">
+      <c r="B24" s="108" t="s">
         <v>15</v>
       </c>
       <c r="C24" s="9" t="s">
@@ -3436,7 +3536,7 @@
       <c r="A25" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="32"/>
+      <c r="B25" s="108"/>
       <c r="C25" s="1" t="s">
         <v>13</v>
       </c>
@@ -3473,7 +3573,7 @@
       <c r="A26" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B26" s="32" t="s">
+      <c r="B26" s="108" t="s">
         <v>60</v>
       </c>
       <c r="C26" s="4" t="s">
@@ -3500,7 +3600,7 @@
       <c r="A27" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B27" s="36"/>
+      <c r="B27" s="107"/>
       <c r="C27" s="3" t="s">
         <v>6</v>
       </c>
@@ -3525,7 +3625,7 @@
       <c r="A28" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B28" s="33" t="s">
+      <c r="B28" s="109" t="s">
         <v>61</v>
       </c>
       <c r="C28" s="3" t="s">
@@ -3552,7 +3652,7 @@
       <c r="A29" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B29" s="32"/>
+      <c r="B29" s="108"/>
       <c r="C29" s="3" t="s">
         <v>6</v>
       </c>
@@ -3575,6 +3675,12 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A18:A23"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="B26:B27"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="A4:A15"/>
     <mergeCell ref="B4:B7"/>
@@ -3591,12 +3697,6 @@
     <mergeCell ref="C12:C15"/>
     <mergeCell ref="D12:D15"/>
     <mergeCell ref="E12:E15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A18:A23"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="B26:B27"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="51" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>